<commit_message>
added white to coding and analyses
</commit_message>
<xml_diff>
--- a/data/otherData/SignProperties.xlsx
+++ b/data/otherData/SignProperties.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgroberts/Documents/MPI/KangSukColours/ColourExperiment/data/otherData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="100">
   <si>
     <t>Sign</t>
   </si>
@@ -310,6 +315,15 @@
   </si>
   <si>
     <t>iconic</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes                                   </t>
+  </si>
+  <si>
+    <t>T0보다 CHECK쪽이 맞음</t>
   </si>
 </sst>
 </file>
@@ -625,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -633,15 +647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="400" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -699,7 +713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -721,7 +735,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -732,7 +746,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -743,7 +757,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -754,7 +768,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -765,7 +779,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -776,7 +790,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -787,7 +801,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -798,7 +812,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -809,7 +823,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -820,7 +834,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -831,7 +845,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -842,7 +856,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -853,7 +867,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -864,7 +878,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -875,7 +889,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -886,7 +900,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -897,7 +911,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -908,7 +922,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -919,7 +933,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -930,7 +944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -941,7 +955,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -952,7 +966,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -963,7 +977,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -974,7 +988,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -985,7 +999,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -996,7 +1010,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1007,7 +1021,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1018,7 +1032,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1029,7 +1043,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1040,7 +1054,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1051,7 +1065,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1062,7 +1076,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1073,7 +1087,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1084,7 +1098,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1095,7 +1109,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1106,7 +1120,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1117,7 +1131,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1128,7 +1142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1139,7 +1153,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1150,7 +1164,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1161,7 +1175,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1172,7 +1186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1183,7 +1197,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1194,7 +1208,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1205,7 +1219,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1216,7 +1230,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1227,7 +1241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1238,7 +1252,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1249,7 +1263,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1260,7 +1274,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1271,7 +1285,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1282,7 +1296,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1293,7 +1307,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1304,7 +1318,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1326,7 +1340,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1337,7 +1351,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1348,7 +1362,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1359,7 +1373,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1370,7 +1384,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1381,7 +1395,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1392,7 +1406,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1403,7 +1417,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1414,7 +1428,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1425,7 +1439,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1436,7 +1450,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1447,7 +1461,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1458,7 +1472,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1469,7 +1483,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -1480,7 +1494,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -1491,7 +1505,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -1502,7 +1516,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1513,7 +1527,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -1535,7 +1549,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -1546,7 +1560,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -1557,7 +1571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -1568,7 +1582,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -1579,7 +1593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -1590,7 +1604,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -1601,7 +1615,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -1612,7 +1626,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -1623,7 +1637,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -1634,7 +1648,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -1645,7 +1659,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -1656,7 +1670,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -1665,6 +1679,28 @@
       </c>
       <c r="C94" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>97</v>
+      </c>
+      <c r="B95" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96" t="s">
+        <v>95</v>
+      </c>
+      <c r="C96" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>